<commit_message>
feat: added seed funders and airdrop allocations
</commit_message>
<xml_diff>
--- a/SNS tokenomics.xlsx
+++ b/SNS tokenomics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\v1ctor\projects\neuralarena-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C07292-A01B-46F8-8BFA-D62DE8AF4CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25A2DB1-1E8C-4B65-8B73-8938483CC341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SNS configuration" sheetId="4" r:id="rId1"/>
@@ -1067,6 +1067,109 @@
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
             <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-0384-4502-9B6D-BAC0A84E7CD3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-0384-4502-9B6D-BAC0A84E7CD3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
                   <a:lumMod val="60000"/>
@@ -1155,9 +1258,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>('Voting power assessment'!$A$12:$A$13,'Voting power assessment'!$A$16,'Voting power assessment'!$A$19)</c:f>
+              <c:f>('Voting power assessment'!$A$12:$A$13,'Voting power assessment'!$A$16:$A$19)</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Decentralization swap - NF</c:v>
                 </c:pt>
@@ -1168,6 +1271,12 @@
                   <c:v>Founding team</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Seed funders</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Airdrop</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Treasury</c:v>
                 </c:pt>
               </c:strCache>
@@ -1182,21 +1291,27 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>('Voting power assessment'!$B$12:$B$13,'Voting power assessment'!$B$16,'Voting power assessment'!$B$19)</c:f>
+              <c:f>('Voting power assessment'!$B$12:$B$13,'Voting power assessment'!$B$16:$B$19)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0;\(#,##0.0\)</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.064516129032258</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.935483870967744</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>61</c:v>
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1270,99 +1385,6 @@
                         <a:gs pos="100000">
                           <a:schemeClr val="accent2">
                             <a:lumMod val="60000"/>
-                            <a:lumMod val="99000"/>
-                            <a:satMod val="120000"/>
-                            <a:shade val="78000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                      </a:gsLst>
-                      <a:lin ang="5400000" scaled="0"/>
-                    </a:gradFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                        <a:srgbClr val="000000">
-                          <a:alpha val="63000"/>
-                        </a:srgbClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c15:spPr>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-                <c15:categoryFilterException>
-                  <c15:sqref>'Voting power assessment'!$B$17</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:gradFill rotWithShape="1">
-                      <a:gsLst>
-                        <a:gs pos="0">
-                          <a:schemeClr val="accent6">
-                            <a:lumMod val="60000"/>
-                            <a:satMod val="103000"/>
-                            <a:lumMod val="102000"/>
-                            <a:tint val="94000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="50000">
-                          <a:schemeClr val="accent6">
-                            <a:lumMod val="60000"/>
-                            <a:satMod val="110000"/>
-                            <a:lumMod val="100000"/>
-                            <a:shade val="100000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="100000">
-                          <a:schemeClr val="accent6">
-                            <a:lumMod val="60000"/>
-                            <a:lumMod val="99000"/>
-                            <a:satMod val="120000"/>
-                            <a:shade val="78000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                      </a:gsLst>
-                      <a:lin ang="5400000" scaled="0"/>
-                    </a:gradFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                        <a:srgbClr val="000000">
-                          <a:alpha val="63000"/>
-                        </a:srgbClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c15:spPr>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-                <c15:categoryFilterException>
-                  <c15:sqref>'Voting power assessment'!$B$18</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:gradFill rotWithShape="1">
-                      <a:gsLst>
-                        <a:gs pos="0">
-                          <a:schemeClr val="accent2">
-                            <a:lumMod val="80000"/>
-                            <a:lumOff val="20000"/>
-                            <a:satMod val="103000"/>
-                            <a:lumMod val="102000"/>
-                            <a:tint val="94000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="50000">
-                          <a:schemeClr val="accent2">
-                            <a:lumMod val="80000"/>
-                            <a:lumOff val="20000"/>
-                            <a:satMod val="110000"/>
-                            <a:lumMod val="100000"/>
-                            <a:shade val="100000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="100000">
-                          <a:schemeClr val="accent2">
-                            <a:lumMod val="80000"/>
-                            <a:lumOff val="20000"/>
                             <a:lumMod val="99000"/>
                             <a:satMod val="120000"/>
                             <a:shade val="78000"/>
@@ -1674,6 +1696,109 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-2A35-4C8D-BC04-B53D8ABBBAFB}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-2A35-4C8D-BC04-B53D8ABBBAFB}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:numFmt formatCode="0.00%" sourceLinked="0"/>
             <c:spPr>
@@ -1740,9 +1865,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>('Voting power assessment'!$A$12:$A$13,'Voting power assessment'!$A$16)</c:f>
+              <c:f>('Voting power assessment'!$A$12:$A$13,'Voting power assessment'!$A$16:$A$18)</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Decentralization swap - NF</c:v>
                 </c:pt>
@@ -1751,6 +1876,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Founding team</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Seed funders</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Airdrop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1764,18 +1895,24 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>('Voting power assessment'!$L$12:$L$13,'Voting power assessment'!$L$16)</c:f>
+              <c:f>('Voting power assessment'!$L$12:$L$13,'Voting power assessment'!$L$16:$L$18)</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.1005296100144439</c:v>
+                  <c:v>0.10713186249358643</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41887337506018296</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.48059701492537316</c:v>
+                  <c:v>0.24781939456131349</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19825551564905078</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3042585941508468E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1849,99 +1986,6 @@
                         <a:gs pos="100000">
                           <a:schemeClr val="accent2">
                             <a:lumMod val="60000"/>
-                            <a:lumMod val="99000"/>
-                            <a:satMod val="120000"/>
-                            <a:shade val="78000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                      </a:gsLst>
-                      <a:lin ang="5400000" scaled="0"/>
-                    </a:gradFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                        <a:srgbClr val="000000">
-                          <a:alpha val="63000"/>
-                        </a:srgbClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c15:spPr>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-                <c15:categoryFilterException>
-                  <c15:sqref>'Voting power assessment'!$L$17</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:gradFill rotWithShape="1">
-                      <a:gsLst>
-                        <a:gs pos="0">
-                          <a:schemeClr val="accent6">
-                            <a:lumMod val="60000"/>
-                            <a:satMod val="103000"/>
-                            <a:lumMod val="102000"/>
-                            <a:tint val="94000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="50000">
-                          <a:schemeClr val="accent6">
-                            <a:lumMod val="60000"/>
-                            <a:satMod val="110000"/>
-                            <a:lumMod val="100000"/>
-                            <a:shade val="100000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="100000">
-                          <a:schemeClr val="accent6">
-                            <a:lumMod val="60000"/>
-                            <a:lumMod val="99000"/>
-                            <a:satMod val="120000"/>
-                            <a:shade val="78000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                      </a:gsLst>
-                      <a:lin ang="5400000" scaled="0"/>
-                    </a:gradFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                        <a:srgbClr val="000000">
-                          <a:alpha val="63000"/>
-                        </a:srgbClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c15:spPr>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-                <c15:categoryFilterException>
-                  <c15:sqref>'Voting power assessment'!$L$18</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:gradFill rotWithShape="1">
-                      <a:gsLst>
-                        <a:gs pos="0">
-                          <a:schemeClr val="accent2">
-                            <a:lumMod val="80000"/>
-                            <a:lumOff val="20000"/>
-                            <a:satMod val="103000"/>
-                            <a:lumMod val="102000"/>
-                            <a:tint val="94000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="50000">
-                          <a:schemeClr val="accent2">
-                            <a:lumMod val="80000"/>
-                            <a:lumOff val="20000"/>
-                            <a:satMod val="110000"/>
-                            <a:lumMod val="100000"/>
-                            <a:shade val="100000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="100000">
-                          <a:schemeClr val="accent2">
-                            <a:lumMod val="80000"/>
-                            <a:lumOff val="20000"/>
                             <a:lumMod val="99000"/>
                             <a:satMod val="120000"/>
                             <a:shade val="78000"/>
@@ -2308,6 +2352,56 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-0AF9-4F0F-BA1E-AA65ED1E5646}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:numFmt formatCode="0.00%" sourceLinked="0"/>
             <c:spPr>
@@ -2374,9 +2468,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>('Voting power assessment'!$A$12,'Voting power assessment'!$A$14,'Voting power assessment'!$A$16)</c:f>
+              <c:f>('Voting power assessment'!$A$12,'Voting power assessment'!$A$14,'Voting power assessment'!$A$16:$A$17)</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Decentralization swap - NF</c:v>
                 </c:pt>
@@ -2385,6 +2479,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Founding team</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Seed funders</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2398,18 +2495,21 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>('Voting power assessment'!$L$12,'Voting power assessment'!$L$14,'Voting power assessment'!$L$16)</c:f>
+              <c:f>('Voting power assessment'!$L$12,'Voting power assessment'!$L$14,'Voting power assessment'!$L$16:$L$17)</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.1005296100144439</c:v>
+                  <c:v>0.10713186249358643</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.4137506413545407</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.48059701492537316</c:v>
+                  <c:v>0.24781939456131349</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19825551564905078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2482,51 +2582,6 @@
                         </a:gs>
                         <a:gs pos="100000">
                           <a:schemeClr val="accent6">
-                            <a:lumMod val="60000"/>
-                            <a:lumMod val="99000"/>
-                            <a:satMod val="120000"/>
-                            <a:shade val="78000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                      </a:gsLst>
-                      <a:lin ang="5400000" scaled="0"/>
-                    </a:gradFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                        <a:srgbClr val="000000">
-                          <a:alpha val="63000"/>
-                        </a:srgbClr>
-                      </a:outerShdw>
-                    </a:effectLst>
-                  </c15:spPr>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-                <c15:categoryFilterException>
-                  <c15:sqref>'Voting power assessment'!$L$17</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:gradFill rotWithShape="1">
-                      <a:gsLst>
-                        <a:gs pos="0">
-                          <a:schemeClr val="accent4">
-                            <a:lumMod val="60000"/>
-                            <a:satMod val="103000"/>
-                            <a:lumMod val="102000"/>
-                            <a:tint val="94000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="50000">
-                          <a:schemeClr val="accent4">
-                            <a:lumMod val="60000"/>
-                            <a:satMod val="110000"/>
-                            <a:lumMod val="100000"/>
-                            <a:shade val="100000"/>
-                          </a:schemeClr>
-                        </a:gs>
-                        <a:gs pos="100000">
-                          <a:schemeClr val="accent4">
                             <a:lumMod val="60000"/>
                             <a:lumMod val="99000"/>
                             <a:satMod val="120000"/>
@@ -3630,7 +3685,7 @@
                 <c:formatCode>#,##0;\(#,##0\)</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>21000000</c:v>
+                  <c:v>28000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3916,10 +3971,10 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>172000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>372000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4021,10 +4076,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.8285714285714282E-2</c:v>
+                  <c:v>4.9999999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.21257142857142858</c:v>
+                  <c:v>9.9999999999999992E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6243,8 +6298,8 @@
   </sheetPr>
   <dimension ref="A1:F1009"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6643,14 +6698,14 @@
         <v>98</v>
       </c>
       <c r="C22" s="69">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="D22" s="65" t="s">
         <v>89</v>
       </c>
       <c r="E22" s="66">
         <f t="shared" si="2"/>
-        <v>10000000000000</v>
+        <v>5000000000000</v>
       </c>
       <c r="F22" s="65" t="s">
         <v>90</v>
@@ -6707,14 +6762,14 @@
         <v>105</v>
       </c>
       <c r="C25" s="69">
-        <v>72000</v>
+        <v>100000</v>
       </c>
       <c r="D25" s="65" t="s">
         <v>89</v>
       </c>
       <c r="E25" s="66">
         <f>C25*10^8</f>
-        <v>7200000000000</v>
+        <v>10000000000000</v>
       </c>
       <c r="F25" s="65" t="s">
         <v>90</v>
@@ -6738,14 +6793,14 @@
         <v>108</v>
       </c>
       <c r="C27" s="70">
-        <v>21000000</v>
+        <v>28000000</v>
       </c>
       <c r="D27" s="65" t="s">
         <v>61</v>
       </c>
       <c r="E27" s="66">
         <f t="shared" ref="E27:E32" si="3">C27*10^8</f>
-        <v>2100000000000000</v>
+        <v>2800000000000000</v>
       </c>
       <c r="F27" s="65" t="s">
         <v>90</v>
@@ -6759,14 +6814,14 @@
         <v>110</v>
       </c>
       <c r="C28" s="70">
-        <v>21000000</v>
+        <v>28000000</v>
       </c>
       <c r="D28" s="65" t="s">
         <v>61</v>
       </c>
       <c r="E28" s="66">
         <f t="shared" si="3"/>
-        <v>2100000000000000</v>
+        <v>2800000000000000</v>
       </c>
       <c r="F28" s="65" t="s">
         <v>90</v>
@@ -6780,14 +6835,14 @@
         <v>112</v>
       </c>
       <c r="C29" s="71">
-        <v>18000000</v>
+        <v>15000000</v>
       </c>
       <c r="D29" s="72" t="s">
         <v>61</v>
       </c>
       <c r="E29" s="73">
         <f t="shared" si="3"/>
-        <v>1800000000000000</v>
+        <v>1500000000000000</v>
       </c>
       <c r="F29" s="72" t="s">
         <v>90</v>
@@ -6801,14 +6856,14 @@
         <v>114</v>
       </c>
       <c r="C30" s="70">
-        <v>0</v>
+        <v>12000000</v>
       </c>
       <c r="D30" s="65" t="s">
         <v>61</v>
       </c>
       <c r="E30" s="66">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1200000000000000</v>
       </c>
       <c r="F30" s="65" t="s">
         <v>90</v>
@@ -6822,14 +6877,14 @@
         <v>116</v>
       </c>
       <c r="C31" s="70">
-        <v>0</v>
+        <v>2000000</v>
       </c>
       <c r="D31" s="65" t="s">
         <v>61</v>
       </c>
       <c r="E31" s="66">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>200000000000000</v>
       </c>
       <c r="F31" s="65" t="s">
         <v>90</v>
@@ -6843,14 +6898,14 @@
         <v>118</v>
       </c>
       <c r="C32" s="70">
-        <v>61000000</v>
+        <v>43000000</v>
       </c>
       <c r="D32" s="65" t="s">
         <v>61</v>
       </c>
       <c r="E32" s="66">
         <f t="shared" si="3"/>
-        <v>6100000000000000</v>
+        <v>4300000000000000</v>
       </c>
       <c r="F32" s="65" t="s">
         <v>90</v>
@@ -6975,7 +7030,7 @@
         <v>126</v>
       </c>
       <c r="B45" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -7046,7 +7101,7 @@
         <v>39</v>
       </c>
       <c r="B54" s="46">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -9933,8 +9988,8 @@
   </sheetPr>
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10024,7 +10079,7 @@
       </c>
       <c r="B7" s="13">
         <f>'SNS configuration'!C25*1/'Token price range'!C6 / 10^6</f>
-        <v>4.064516129032258</v>
+        <v>7</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -10044,7 +10099,7 @@
       </c>
       <c r="B8" s="14">
         <f>'SNS configuration'!C28/10^6</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -10064,7 +10119,7 @@
       </c>
       <c r="B9" s="13">
         <f>B8-B7</f>
-        <v>16.935483870967744</v>
+        <v>21</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -10151,7 +10206,7 @@
       </c>
       <c r="B12" s="18">
         <f>B7</f>
-        <v>4.064516129032258</v>
+        <v>7</v>
       </c>
       <c r="C12" s="19">
         <f>'SNS configuration'!B38</f>
@@ -10159,7 +10214,7 @@
       </c>
       <c r="D12" s="20">
         <f t="shared" ref="D12:D19" si="0">B12*C12</f>
-        <v>3.4838709677419351</v>
+        <v>6</v>
       </c>
       <c r="E12" s="21">
         <f>'SNS configuration'!C38</f>
@@ -10174,11 +10229,11 @@
       </c>
       <c r="H12" s="20">
         <f t="shared" ref="H12:H14" si="2">D12*F12*G12</f>
-        <v>3.7887096774193543</v>
+        <v>6.5249999999999995</v>
       </c>
       <c r="I12" s="22">
         <f t="shared" ref="I12:I19" si="3">H12/$H$20</f>
-        <v>0.1005296100144439</v>
+        <v>0.10713186249358643</v>
       </c>
       <c r="J12" s="19">
         <f>IF( 'SNS configuration'!$B$45, 'SNS configuration'!B50, 100%)</f>
@@ -10186,11 +10241,11 @@
       </c>
       <c r="K12" s="20">
         <f t="shared" ref="K12:K14" si="4">H12*J12</f>
-        <v>3.7887096774193543</v>
+        <v>6.5249999999999995</v>
       </c>
       <c r="L12" s="78">
         <f t="shared" ref="L12:L19" si="5">K12/$K$20</f>
-        <v>0.1005296100144439</v>
+        <v>0.10713186249358643</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
@@ -10199,7 +10254,7 @@
       </c>
       <c r="B13" s="18">
         <f>IF('SNS configuration'!B45, (1-'SNS configuration'!B46)*B9, B9)</f>
-        <v>16.935483870967744</v>
+        <v>0</v>
       </c>
       <c r="C13" s="19">
         <f>'SNS configuration'!B39</f>
@@ -10207,7 +10262,7 @@
       </c>
       <c r="D13" s="20">
         <f t="shared" si="0"/>
-        <v>14.516129032258066</v>
+        <v>0</v>
       </c>
       <c r="E13" s="21">
         <f>'SNS configuration'!C39</f>
@@ -10222,11 +10277,11 @@
       </c>
       <c r="H13" s="20">
         <f t="shared" si="2"/>
-        <v>15.786290322580646</v>
+        <v>0</v>
       </c>
       <c r="I13" s="22">
         <f t="shared" si="3"/>
-        <v>0.41887337506018296</v>
+        <v>0</v>
       </c>
       <c r="J13" s="19">
         <f>IF( 'SNS configuration'!$B$45, 'SNS configuration'!B51, 100%)</f>
@@ -10234,11 +10289,11 @@
       </c>
       <c r="K13" s="20">
         <f t="shared" si="4"/>
-        <v>15.786290322580646</v>
+        <v>0</v>
       </c>
       <c r="L13" s="78">
         <f t="shared" si="5"/>
-        <v>0.41887337506018296</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
@@ -10247,7 +10302,7 @@
       </c>
       <c r="B14" s="18">
         <f>IF('SNS configuration'!B45, 'SNS configuration'!B46*B9, 0)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C14" s="19">
         <f>'SNS configuration'!B47</f>
@@ -10255,7 +10310,7 @@
       </c>
       <c r="D14" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E14" s="7">
         <f>'SNS configuration'!B48</f>
@@ -10270,11 +10325,11 @@
       </c>
       <c r="H14" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>25.2</v>
       </c>
       <c r="I14" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.4137506413545407</v>
       </c>
       <c r="J14" s="19">
         <f>IF( 'SNS configuration'!$B$45, 'SNS configuration'!B52, 100%)</f>
@@ -10282,11 +10337,11 @@
       </c>
       <c r="K14" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>25.2</v>
       </c>
       <c r="L14" s="78">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.4137506413545407</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
@@ -10325,7 +10380,7 @@
       </c>
       <c r="B16" s="18">
         <f>'SNS configuration'!C29/10^6</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C16" s="19">
         <f>'SNS configuration'!B40</f>
@@ -10333,7 +10388,7 @@
       </c>
       <c r="D16" s="20">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E16" s="21">
         <f>'SNS configuration'!C40</f>
@@ -10349,11 +10404,11 @@
       </c>
       <c r="H16" s="20">
         <f t="shared" ref="H16:H18" si="7">D16*F16*G16</f>
-        <v>18.112500000000001</v>
+        <v>15.093750000000002</v>
       </c>
       <c r="I16" s="22">
         <f t="shared" si="3"/>
-        <v>0.48059701492537316</v>
+        <v>0.24781939456131349</v>
       </c>
       <c r="J16" s="19">
         <f>IF( 'SNS configuration'!$B$45, 'SNS configuration'!B52, 100%)</f>
@@ -10361,11 +10416,11 @@
       </c>
       <c r="K16" s="20">
         <f t="shared" ref="K16:K18" si="8">H16*J16</f>
-        <v>18.112500000000001</v>
+        <v>15.093750000000002</v>
       </c>
       <c r="L16" s="78">
         <f t="shared" si="5"/>
-        <v>0.48059701492537316</v>
+        <v>0.24781939456131349</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -10374,7 +10429,7 @@
       </c>
       <c r="B17" s="18">
         <f>'SNS configuration'!C30/10^6</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C17" s="19">
         <f>'SNS configuration'!B41</f>
@@ -10382,7 +10437,7 @@
       </c>
       <c r="D17" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E17" s="21">
         <f>'SNS configuration'!C41</f>
@@ -10398,11 +10453,11 @@
       </c>
       <c r="H17" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>12.075000000000001</v>
       </c>
       <c r="I17" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.19825551564905078</v>
       </c>
       <c r="J17" s="19">
         <f>IF( 'SNS configuration'!$B$45, 'SNS configuration'!B53, 100%)</f>
@@ -10410,11 +10465,11 @@
       </c>
       <c r="K17" s="20">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>12.075000000000001</v>
       </c>
       <c r="L17" s="78">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.19825551564905078</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -10423,7 +10478,7 @@
       </c>
       <c r="B18" s="18">
         <f>'SNS configuration'!C31/10^6</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C18" s="19">
         <f>'SNS configuration'!B42</f>
@@ -10431,7 +10486,7 @@
       </c>
       <c r="D18" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="21">
         <f>'SNS configuration'!C42</f>
@@ -10446,11 +10501,11 @@
       </c>
       <c r="H18" s="20">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2.0125000000000002</v>
       </c>
       <c r="I18" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.3042585941508468E-2</v>
       </c>
       <c r="J18" s="19">
         <f>IF( 'SNS configuration'!$B$45, 'SNS configuration'!B54, 100%)</f>
@@ -10458,11 +10513,11 @@
       </c>
       <c r="K18" s="20">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2.0125000000000002</v>
       </c>
       <c r="L18" s="78">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.3042585941508468E-2</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -10471,7 +10526,7 @@
       </c>
       <c r="B19" s="18">
         <f>'SNS configuration'!C32/10^6</f>
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C19" s="19">
         <v>0</v>
@@ -10506,14 +10561,14 @@
       <c r="C20" s="7"/>
       <c r="D20" s="20">
         <f>SUM(D12:D19)</f>
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="20">
         <f>SUM(H12:H19)</f>
-        <v>37.6875</v>
+        <v>60.906250000000007</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7">
@@ -10522,7 +10577,7 @@
       </c>
       <c r="K20" s="20">
         <f>SUM(K12:K19)</f>
-        <v>37.6875</v>
+        <v>60.906250000000007</v>
       </c>
       <c r="L20" s="23"/>
     </row>
@@ -10988,8 +11043,8 @@
   </sheetPr>
   <dimension ref="A2:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11006,7 +11061,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -11033,23 +11088,23 @@
       </c>
       <c r="B5" s="3">
         <f>'SNS configuration'!C18+'SNS configuration'!C25</f>
-        <v>172000</v>
+        <v>200000</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" ref="C5:C6" si="0">B5/$B$7</f>
-        <v>8.1904761904761907E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" ref="D5:D6" si="1">C5*$B$2</f>
-        <v>9.8285714285714282E-2</v>
+        <v>4.9999999999999996E-2</v>
       </c>
       <c r="E5" s="81">
         <f>$B5*(('SNS configuration'!$C$33)/$B$7)</f>
-        <v>819047.61904761905</v>
+        <v>714285.71428571432</v>
       </c>
       <c r="F5" s="80">
         <f>E5*$B$2</f>
-        <v>9828571.4285714291</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -11058,23 +11113,23 @@
       </c>
       <c r="B6" s="3">
         <f>'SNS configuration'!C19+'SNS configuration'!C25</f>
-        <v>372000</v>
+        <v>400000</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>1.7714285714285714E-2</v>
+        <v>1.4285714285714285E-2</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="1"/>
-        <v>0.21257142857142858</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="E6" s="81">
         <f>$B6*(('SNS configuration'!$C$33)/$B$7)</f>
-        <v>1771428.5714285714</v>
+        <v>1428571.4285714286</v>
       </c>
       <c r="F6" s="80">
         <f>E6*$B$2</f>
-        <v>21257142.857142858</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -11083,7 +11138,7 @@
       </c>
       <c r="B7" s="5">
         <f>'SNS configuration'!C28</f>
-        <v>21000000</v>
+        <v>28000000</v>
       </c>
       <c r="D7" s="6">
         <f>D11</f>
@@ -11115,7 +11170,7 @@
       </c>
       <c r="B32" s="7">
         <f>B31/'Token price range'!C6</f>
-        <v>56.451612903225808</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -11142,7 +11197,7 @@
       </c>
       <c r="B35" s="7">
         <f>B32/B33-B34</f>
-        <v>8.0545161290322582</v>
+        <v>9.99</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>